<commit_message>
add groups to sites report template
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/site_report_template.xlsx
+++ b/bio_diversity/static/report_templates/site_report_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Release Site Name</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>End Date</t>
+  </si>
+  <si>
+    <t>Group</t>
   </si>
 </sst>
 </file>
@@ -894,10 +897,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,21 +908,21 @@
     <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="4" max="5" width="15.28515625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="1"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="2"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="2"/>
+      <c r="H1" s="3"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -927,19 +930,20 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="4"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -952,10 +956,13 @@
       <c r="D3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
clean up site reports
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/site_report_template.xlsx
+++ b/bio_diversity/static/report_templates/site_report_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Release Site Name</t>
   </si>
@@ -45,7 +45,10 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>Group</t>
+    <t>Program Group</t>
+  </si>
+  <si>
+    <t>Collection</t>
   </si>
 </sst>
 </file>
@@ -897,7 +900,7 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
@@ -908,11 +911,12 @@
     <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.28515625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="7" customWidth="1"/>
+    <col min="5" max="6" width="26.5703125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -920,10 +924,10 @@
       <c r="C1" s="1"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="2"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="2"/>
+      <c r="I1" s="3"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -931,19 +935,20 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="4"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -957,12 +962,15 @@
         <v>3</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add individual details to sites report, #831
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/site_report_template.xlsx
+++ b/bio_diversity/static/report_templates/site_report_template.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="template" sheetId="3" r:id="rId1"/>
+    <sheet name="Sites" sheetId="3" r:id="rId1"/>
+    <sheet name="Individuals" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Release Site Name</t>
   </si>
@@ -49,14 +50,45 @@
   </si>
   <si>
     <t>Collection</t>
+  </si>
+  <si>
+    <t>PIT Tag</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Lifestage</t>
+  </si>
+  <si>
+    <t>Site Name</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Weight (g)</t>
+  </si>
+  <si>
+    <t>Length (cm)</t>
+  </si>
+  <si>
+    <t>End:</t>
+  </si>
+  <si>
+    <t>Start:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -382,7 +414,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -497,6 +529,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -542,16 +583,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -902,8 +944,8 @@
   </sheetPr>
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,8 +953,8 @@
     <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="7" customWidth="1"/>
-    <col min="5" max="6" width="26.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="6" customWidth="1"/>
+    <col min="5" max="6" width="26.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -922,9 +964,9 @@
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
       <c r="G1" s="2"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -948,14 +990,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -967,12 +1009,89 @@
       <c r="F3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="8" t="s">
         <v>5</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G4" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
start adding distributions and collections tabs to sites report
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/site_report_template.xlsx
+++ b/bio_diversity/static/report_templates/site_report_template.xlsx
@@ -9,18 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sites" sheetId="3" r:id="rId1"/>
     <sheet name="Individuals" sheetId="4" r:id="rId2"/>
+    <sheet name="Collections" sheetId="5" r:id="rId3"/>
+    <sheet name="Distributions" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="27">
   <si>
     <t>Release Site Name</t>
   </si>
@@ -89,6 +91,18 @@
   </si>
   <si>
     <t>Weight(g)</t>
+  </si>
+  <si>
+    <t>Release Method</t>
+  </si>
+  <si>
+    <t>Truck Temp</t>
+  </si>
+  <si>
+    <t>River Temp</t>
+  </si>
+  <si>
+    <t>Acclimation Time (mins)</t>
   </si>
 </sst>
 </file>
@@ -953,8 +967,8 @@
   </sheetPr>
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,4 +1130,226 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" customWidth="1"/>
+    <col min="16" max="16" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add links expand distributions tab on sites report
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/site_report_template.xlsx
+++ b/bio_diversity/static/report_templates/site_report_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sites" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
   <si>
     <t>Release Site Name</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Acclimation Time (mins)</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
@@ -965,10 +968,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,10 +981,9 @@
     <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" style="6" customWidth="1"/>
     <col min="5" max="7" width="26.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -992,29 +994,25 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="O1" s="4"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
-      <c r="S1" s="4"/>
+      <c r="S1" s="2"/>
       <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1037,16 +1035,7 @@
         <v>20</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1136,7 +1125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1235,33 +1224,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" customWidth="1"/>
-    <col min="16" max="16" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" customWidth="1"/>
+    <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" customWidth="1"/>
+    <col min="17" max="17" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1271,25 +1261,26 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="4"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1297,8 +1288,9 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1321,30 +1313,33 @@
         <v>20</v>
       </c>
       <c r="H3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="M3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="8" t="s">
+      <c r="N3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="Q3" s="7" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add colections tab to sites report
</commit_message>
<xml_diff>
--- a/bio_diversity/static/report_templates/site_report_template.xlsx
+++ b/bio_diversity/static/report_templates/site_report_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sites" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
   <si>
     <t>Release Site Name</t>
   </si>
@@ -1123,10 +1123,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,14 +1137,14 @@
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="7" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1154,10 +1154,10 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="2"/>
       <c r="J1" s="3"/>
-      <c r="K1" s="2"/>
+      <c r="K1" s="3"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -1165,14 +1165,15 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="4"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1180,8 +1181,9 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1204,16 +1206,22 @@
         <v>20</v>
       </c>
       <c r="H3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>22</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1226,7 +1234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>

</xml_diff>